<commit_message>
se agrega spectral clustering
</commit_message>
<xml_diff>
--- a/GMMHMM/grupo1/X_test.xlsx
+++ b/GMMHMM/grupo1/X_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>RMS</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>ADIm11</t>
+  </si>
+  <si>
+    <t>target</t>
   </si>
 </sst>
 </file>
@@ -456,144 +459,146 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>0.085567775</v>
+        <v>1.088576992162783</v>
       </c>
       <c r="C2">
-        <v>0.159892869</v>
+        <v>1.113879672048004</v>
       </c>
       <c r="D2">
-        <v>1.302214989</v>
+        <v>1.391852302160855</v>
       </c>
       <c r="E2">
-        <v>1.364631935</v>
+        <v>1.097675066956605</v>
       </c>
       <c r="F2">
-        <v>1.485582903</v>
+        <v>0.6193999948385083</v>
       </c>
       <c r="G2">
-        <v>1.670552813</v>
+        <v>1.260478162207732</v>
       </c>
       <c r="H2">
-        <v>1.375458835</v>
+        <v>0.2829759842181138</v>
       </c>
       <c r="I2">
-        <v>1.598300127</v>
+        <v>-0.2048732487660765</v>
       </c>
       <c r="J2">
-        <v>1.573589684</v>
+        <v>1.280068775920671</v>
       </c>
       <c r="K2">
-        <v>1.107643066</v>
+        <v>0.4598623887690349</v>
       </c>
       <c r="L2">
-        <v>0.357598597</v>
+        <v>0.7524404323814086</v>
       </c>
       <c r="M2">
-        <v>0.239382497</v>
+        <v>0.802791065925304</v>
       </c>
       <c r="N2">
-        <v>0.103043273</v>
+        <v>0.7880756782855436</v>
       </c>
       <c r="O2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>-1.010591776</v>
+        <v>-1.052360446</v>
       </c>
       <c r="C3">
-        <v>-1.054430187</v>
+        <v>-1.116420485</v>
       </c>
       <c r="D3">
-        <v>-0.475581808</v>
+        <v>-1.102244233</v>
       </c>
       <c r="E3">
-        <v>-0.928587107</v>
+        <v>-2.994605003</v>
       </c>
       <c r="F3">
-        <v>-0.649071957</v>
+        <v>-2.034215286</v>
       </c>
       <c r="G3">
-        <v>-0.510664725</v>
+        <v>-1.796524334</v>
       </c>
       <c r="H3">
-        <v>-1.155691688</v>
+        <v>-1.041387772</v>
       </c>
       <c r="I3">
-        <v>-0.136370929</v>
+        <v>-0.212968827</v>
       </c>
       <c r="J3">
-        <v>0.13459405</v>
+        <v>0.294011831</v>
       </c>
       <c r="K3">
-        <v>3.63e-05</v>
+        <v>0.103498634</v>
       </c>
       <c r="L3">
-        <v>-0.438832638</v>
+        <v>-0.09137593400000001</v>
       </c>
       <c r="M3">
-        <v>-0.356669814</v>
+        <v>-0.624227593</v>
       </c>
       <c r="N3">
-        <v>-0.026622818</v>
+        <v>-0.321369264</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B4">
-        <v>0.068718052</v>
+        <v>-0.9673902202431353</v>
       </c>
       <c r="C4">
-        <v>0.135924307</v>
+        <v>-1.005585475346329</v>
       </c>
       <c r="D4">
-        <v>-0.397392081</v>
+        <v>0.01336928259588351</v>
       </c>
       <c r="E4">
-        <v>-1.031961151</v>
+        <v>-0.03144927010491952</v>
       </c>
       <c r="F4">
-        <v>-0.153897081</v>
+        <v>-0.8290864447953518</v>
       </c>
       <c r="G4">
-        <v>0.141923944</v>
+        <v>-0.3559431232112886</v>
       </c>
       <c r="H4">
-        <v>-0.09817292</v>
+        <v>-1.188186603427425</v>
       </c>
       <c r="I4">
-        <v>0.027253499</v>
+        <v>-2.503584584696504</v>
       </c>
       <c r="J4">
-        <v>0.300797822</v>
+        <v>-2.388757987935037</v>
       </c>
       <c r="K4">
-        <v>0.373804826</v>
+        <v>-1.560003476310523</v>
       </c>
       <c r="L4">
-        <v>-0.9805031190000001</v>
+        <v>-0.9705462612823146</v>
       </c>
       <c r="M4">
-        <v>-0.9644059559999999</v>
+        <v>-0.4379119648592557</v>
       </c>
       <c r="N4">
-        <v>-0.7646438</v>
+        <v>-0.6418788257929507</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -601,46 +606,46 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>0.097755729</v>
+        <v>1.09260717879037</v>
       </c>
       <c r="C5">
-        <v>0.150196918</v>
+        <v>1.10528016275872</v>
       </c>
       <c r="D5">
-        <v>-0.670648536</v>
+        <v>-0.5052371728717996</v>
       </c>
       <c r="E5">
-        <v>-1.593252783</v>
+        <v>-1.213035656723745</v>
       </c>
       <c r="F5">
-        <v>-1.829066919</v>
+        <v>-0.9397964201281946</v>
       </c>
       <c r="G5">
-        <v>-0.082484553</v>
+        <v>-0.07632542278754005</v>
       </c>
       <c r="H5">
-        <v>-0.213239198</v>
+        <v>-0.1814666348577954</v>
       </c>
       <c r="I5">
-        <v>-0.003668579</v>
+        <v>-0.08897598996320968</v>
       </c>
       <c r="J5">
-        <v>-0.194428542</v>
+        <v>-0.1461574093903557</v>
       </c>
       <c r="K5">
-        <v>-0.929000237</v>
+        <v>-0.5692170635129519</v>
       </c>
       <c r="L5">
-        <v>-2.715263813</v>
+        <v>-1.400241450620395</v>
       </c>
       <c r="M5">
-        <v>-3.459791333</v>
+        <v>-1.52723548122241</v>
       </c>
       <c r="N5">
-        <v>-3.414935158</v>
+        <v>-1.861333063595394</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -648,140 +653,140 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>0.09273416400000001</v>
+        <v>1.168895327646786</v>
       </c>
       <c r="C6">
-        <v>0.167730306</v>
+        <v>1.124790058217134</v>
       </c>
       <c r="D6">
-        <v>1.336888192</v>
+        <v>-0.108837563652328</v>
       </c>
       <c r="E6">
-        <v>1.37678494</v>
+        <v>-0.527461071075682</v>
       </c>
       <c r="F6">
-        <v>1.727839705</v>
+        <v>-0.8652942322810397</v>
       </c>
       <c r="G6">
-        <v>1.780657985</v>
+        <v>0.1168204941201648</v>
       </c>
       <c r="H6">
-        <v>1.71084308</v>
+        <v>-0.723641543470295</v>
       </c>
       <c r="I6">
-        <v>1.737646294</v>
+        <v>-0.498731630075758</v>
       </c>
       <c r="J6">
-        <v>1.672063467</v>
+        <v>-1.025476842083122</v>
       </c>
       <c r="K6">
-        <v>2.101930869</v>
+        <v>-1.622354741293647</v>
       </c>
       <c r="L6">
-        <v>1.598622792</v>
+        <v>-2.117899344682976</v>
       </c>
       <c r="M6">
-        <v>1.344010916</v>
+        <v>-2.105917768685274</v>
       </c>
       <c r="N6">
-        <v>1.350692732</v>
+        <v>-2.604525295334807</v>
       </c>
       <c r="O6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="B7">
-        <v>-0.94446379</v>
+        <v>-0.9801136137722205</v>
       </c>
       <c r="C7">
-        <v>-1.03312062</v>
+        <v>-1.041956232283092</v>
       </c>
       <c r="D7">
-        <v>-0.276982851</v>
+        <v>-0.1886708569035639</v>
       </c>
       <c r="E7">
-        <v>-0.9703883059999999</v>
+        <v>0.03187326138358325</v>
       </c>
       <c r="F7">
-        <v>-0.8156206640000001</v>
+        <v>0.02696679057833097</v>
       </c>
       <c r="G7">
-        <v>-1.50879384</v>
+        <v>0.4139021714331789</v>
       </c>
       <c r="H7">
-        <v>-0.9600969540000001</v>
+        <v>-0.2537263285459994</v>
       </c>
       <c r="I7">
-        <v>-0.278943511</v>
+        <v>-0.7238580530731326</v>
       </c>
       <c r="J7">
-        <v>-0.470813446</v>
+        <v>-0.8867859043564654</v>
       </c>
       <c r="K7">
-        <v>0.004103698</v>
+        <v>-0.4421644275965932</v>
       </c>
       <c r="L7">
-        <v>-0.340909939</v>
+        <v>0.5141295735833261</v>
       </c>
       <c r="M7">
-        <v>-0.297489162</v>
+        <v>0.4309079702258571</v>
       </c>
       <c r="N7">
-        <v>0.09127224099999999</v>
+        <v>0.6473643899869618</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>-1.172068029</v>
+        <v>1.200056980136892</v>
       </c>
       <c r="C8">
-        <v>-1.231346413</v>
+        <v>1.123243570411099</v>
       </c>
       <c r="D8">
-        <v>-0.415498974</v>
+        <v>-0.55241059474163</v>
       </c>
       <c r="E8">
-        <v>-0.528098325</v>
+        <v>-1.036721346042088</v>
       </c>
       <c r="F8">
-        <v>-0.319651611</v>
+        <v>-0.9308365164426041</v>
       </c>
       <c r="G8">
-        <v>0.629820739</v>
+        <v>0.1155780199142884</v>
       </c>
       <c r="H8">
-        <v>-0.400841936</v>
+        <v>0.2663936930680734</v>
       </c>
       <c r="I8">
-        <v>-0.295586328</v>
+        <v>0.02870485741260834</v>
       </c>
       <c r="J8">
-        <v>-0.298862914</v>
+        <v>-0.602788081833072</v>
       </c>
       <c r="K8">
-        <v>0.279929195</v>
+        <v>-1.192180913668596</v>
       </c>
       <c r="L8">
-        <v>0.281425611</v>
+        <v>-2.247474818272565</v>
       </c>
       <c r="M8">
-        <v>0.266629758</v>
+        <v>-2.537178146746713</v>
       </c>
       <c r="N8">
-        <v>0.546506038</v>
+        <v>-2.569831016425473</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -789,46 +794,46 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>-0.910313292</v>
+        <v>0.09099733199999999</v>
       </c>
       <c r="C9">
-        <v>-1.15848515</v>
+        <v>0.165123739</v>
       </c>
       <c r="D9">
-        <v>-1.259229058</v>
+        <v>1.033777922</v>
       </c>
       <c r="E9">
-        <v>-0.805998625</v>
+        <v>0.62781765</v>
       </c>
       <c r="F9">
-        <v>-0.358941927</v>
+        <v>0.7088679729999999</v>
       </c>
       <c r="G9">
-        <v>0.325726794</v>
+        <v>0.9639872290000001</v>
       </c>
       <c r="H9">
-        <v>-0.247567924</v>
+        <v>-0.570432089</v>
       </c>
       <c r="I9">
-        <v>-0.9535645699999999</v>
+        <v>-0.6886823870000001</v>
       </c>
       <c r="J9">
-        <v>-0.379365554</v>
+        <v>-0.226930379</v>
       </c>
       <c r="K9">
-        <v>-0.669414201</v>
+        <v>0.2216372</v>
       </c>
       <c r="L9">
-        <v>0.05102243099999999</v>
+        <v>-0.154145444</v>
       </c>
       <c r="M9">
-        <v>0.189273845</v>
+        <v>0.244069248</v>
       </c>
       <c r="N9">
-        <v>0.361967262</v>
+        <v>0.37543717</v>
       </c>
       <c r="O9">
         <v>1</v>
@@ -836,422 +841,422 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="1">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="B10">
-        <v>-0.8492548329999999</v>
+        <v>-1.053461550083322</v>
       </c>
       <c r="C10">
-        <v>-0.8901110990000001</v>
+        <v>-1.013951085727377</v>
       </c>
       <c r="D10">
-        <v>-0.113791962</v>
+        <v>-1.670975857646011</v>
       </c>
       <c r="E10">
-        <v>0.696699691</v>
+        <v>-2.305474877223224</v>
       </c>
       <c r="F10">
-        <v>1.330175595</v>
+        <v>-1.061541930846145</v>
       </c>
       <c r="G10">
-        <v>0.55119769</v>
+        <v>-1.097802694772028</v>
       </c>
       <c r="H10">
-        <v>1.259601198</v>
+        <v>-0.2332301376733607</v>
       </c>
       <c r="I10">
-        <v>1.053115556</v>
+        <v>0.2441601328574322</v>
       </c>
       <c r="J10">
-        <v>0.915666889</v>
+        <v>0.3523387254212044</v>
       </c>
       <c r="K10">
-        <v>1.195823559</v>
+        <v>-0.2489324891736348</v>
       </c>
       <c r="L10">
-        <v>1.10706505</v>
+        <v>-0.502001930595651</v>
       </c>
       <c r="M10">
-        <v>0.95634344</v>
+        <v>-0.6653240106200277</v>
       </c>
       <c r="N10">
-        <v>0.80150649</v>
+        <v>-0.3590114128251046</v>
       </c>
       <c r="O10">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>0.080138772</v>
+        <v>0.08650412199999999</v>
       </c>
       <c r="C11">
-        <v>0.152574184</v>
+        <v>0.16076415</v>
       </c>
       <c r="D11">
-        <v>1.080125462</v>
+        <v>1.287529653</v>
       </c>
       <c r="E11">
-        <v>0.455753224</v>
+        <v>1.458507674</v>
       </c>
       <c r="F11">
-        <v>-0.494340361</v>
+        <v>1.708264452</v>
       </c>
       <c r="G11">
-        <v>0.115745779</v>
+        <v>1.737302749</v>
       </c>
       <c r="H11">
-        <v>-1.64103004</v>
+        <v>1.454654867</v>
       </c>
       <c r="I11">
-        <v>-1.689385246</v>
+        <v>1.685926169</v>
       </c>
       <c r="J11">
-        <v>-0.9455622859999999</v>
+        <v>1.198936477</v>
       </c>
       <c r="K11">
-        <v>-0.857492658</v>
+        <v>1.009485194</v>
       </c>
       <c r="L11">
-        <v>-1.499750307</v>
+        <v>0.6228660539999999</v>
       </c>
       <c r="M11">
-        <v>-0.505977107</v>
+        <v>0.391809069</v>
       </c>
       <c r="N11">
-        <v>-0.66795561</v>
+        <v>0.180105296</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="1">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B12">
-        <v>-1.075959248</v>
+        <v>-0.915313197917203</v>
       </c>
       <c r="C12">
-        <v>-1.148089415</v>
+        <v>-0.8002599253251903</v>
       </c>
       <c r="D12">
-        <v>-1.29033459</v>
+        <v>-0.4858008915469419</v>
       </c>
       <c r="E12">
-        <v>-0.4561949702537312</v>
+        <v>-0.459102613136871</v>
       </c>
       <c r="F12">
-        <v>-1.658406479</v>
+        <v>-0.3886572214119309</v>
       </c>
       <c r="G12">
-        <v>-0.478718335</v>
+        <v>-1.131570294461621</v>
       </c>
       <c r="H12">
-        <v>-0.405491016</v>
+        <v>-0.4310121901661068</v>
       </c>
       <c r="I12">
-        <v>-0.294614211</v>
+        <v>0.1352166989295445</v>
       </c>
       <c r="J12">
-        <v>-0.097444049</v>
+        <v>0.0321162105799529</v>
       </c>
       <c r="K12">
-        <v>-0.581121552</v>
+        <v>0.2689214043482228</v>
       </c>
       <c r="L12">
-        <v>-1.390411525</v>
+        <v>0.1719394788427852</v>
       </c>
       <c r="M12">
-        <v>-1.808725387</v>
+        <v>0.01614742187502364</v>
       </c>
       <c r="N12">
-        <v>-1.013263883</v>
+        <v>0.2079486552789812</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="1">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B13">
-        <v>-1.042198087</v>
+        <v>-0.5773369837013437</v>
       </c>
       <c r="C13">
-        <v>-1.196787822</v>
+        <v>-0.7008086824709544</v>
       </c>
       <c r="D13">
-        <v>-0.4783288429999999</v>
+        <v>-1.04388155837972</v>
       </c>
       <c r="E13">
-        <v>-0.29351785</v>
+        <v>-0.889075565958088</v>
       </c>
       <c r="F13">
-        <v>0.07789871299999999</v>
+        <v>-0.4777298958116295</v>
       </c>
       <c r="G13">
-        <v>0.589451356</v>
+        <v>-0.7205425914449428</v>
       </c>
       <c r="H13">
-        <v>-0.249145236</v>
+        <v>-0.7971610748256895</v>
       </c>
       <c r="I13">
-        <v>-0.273429519</v>
+        <v>-0.008196996251951846</v>
       </c>
       <c r="J13">
-        <v>-0.084926801</v>
+        <v>-1.049105483397343</v>
       </c>
       <c r="K13">
-        <v>-0.34367782</v>
+        <v>-0.1228300179444196</v>
       </c>
       <c r="L13">
-        <v>0.118776451</v>
+        <v>0.0830021749573447</v>
       </c>
       <c r="M13">
-        <v>0.012452516</v>
+        <v>0.2045357481978724</v>
       </c>
       <c r="N13">
-        <v>0.271643513</v>
+        <v>0.269263486568356</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="1">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B14">
-        <v>0.084514785</v>
+        <v>-0.8999088371623735</v>
       </c>
       <c r="C14">
-        <v>0.158664541</v>
+        <v>-0.7979083676895516</v>
       </c>
       <c r="D14">
-        <v>1.255127339</v>
+        <v>-0.3777293800015497</v>
       </c>
       <c r="E14">
-        <v>1.338850758</v>
+        <v>-0.4738492208868103</v>
       </c>
       <c r="F14">
-        <v>1.651653511</v>
+        <v>-0.4220898121785666</v>
       </c>
       <c r="G14">
-        <v>1.838477983</v>
+        <v>-0.6004718027471426</v>
       </c>
       <c r="H14">
-        <v>1.76996833</v>
+        <v>-1.011272578681248</v>
       </c>
       <c r="I14">
-        <v>1.724213095</v>
+        <v>0.1028459493065351</v>
       </c>
       <c r="J14">
-        <v>1.669531759</v>
+        <v>0.3114022967378419</v>
       </c>
       <c r="K14">
-        <v>1.780583401</v>
+        <v>0.1371577873176834</v>
       </c>
       <c r="L14">
-        <v>1.244663889</v>
+        <v>-0.03766079638830301</v>
       </c>
       <c r="M14">
-        <v>0.8648448559999999</v>
+        <v>0.1002645347072279</v>
       </c>
       <c r="N14">
-        <v>0.839562017</v>
+        <v>0.2894954110783645</v>
       </c>
       <c r="O14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>-1.113243525</v>
+        <v>-0.9819434020000001</v>
       </c>
       <c r="C15">
-        <v>-1.218439747</v>
+        <v>-1.027168868</v>
       </c>
       <c r="D15">
-        <v>-0.46169408</v>
+        <v>-0.391420759</v>
       </c>
       <c r="E15">
-        <v>-0.506681916</v>
+        <v>-1.071957494</v>
       </c>
       <c r="F15">
-        <v>-0.141881335</v>
+        <v>-1.015058936</v>
       </c>
       <c r="G15">
-        <v>0.22744881</v>
+        <v>-1.251488744</v>
       </c>
       <c r="H15">
-        <v>-0.997138382</v>
+        <v>-1.889056123</v>
       </c>
       <c r="I15">
-        <v>-1.313530996</v>
+        <v>-0.649593132</v>
       </c>
       <c r="J15">
-        <v>-0.829717461</v>
+        <v>-0.321722455</v>
       </c>
       <c r="K15">
-        <v>-0.556270676</v>
+        <v>-0.310259495</v>
       </c>
       <c r="L15">
-        <v>-0.016803582</v>
+        <v>-0.362302266</v>
       </c>
       <c r="M15">
-        <v>-0.136466835</v>
+        <v>-0.24811692</v>
       </c>
       <c r="N15">
-        <v>0.219988164</v>
+        <v>0.142904433</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="1">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B16">
-        <v>-1.162809267</v>
+        <v>-0.4486676309063777</v>
       </c>
       <c r="C16">
-        <v>-1.230742598</v>
+        <v>-0.6981368151440918</v>
       </c>
       <c r="D16">
-        <v>-0.481548895</v>
+        <v>-1.893864632384399</v>
       </c>
       <c r="E16">
-        <v>-0.48584958</v>
+        <v>-0.8138407903746437</v>
       </c>
       <c r="F16">
-        <v>-0.43719234</v>
+        <v>-1.131585928047311</v>
       </c>
       <c r="G16">
-        <v>0.114115978</v>
+        <v>-1.521676146207622</v>
       </c>
       <c r="H16">
-        <v>-0.77417708</v>
+        <v>-0.421539501489349</v>
       </c>
       <c r="I16">
-        <v>-1.367703306</v>
+        <v>-0.9139190013134963</v>
       </c>
       <c r="J16">
-        <v>-0.7770090820000001</v>
+        <v>0.078154540762746</v>
       </c>
       <c r="K16">
-        <v>-0.805050077</v>
+        <v>-0.03860679876158272</v>
       </c>
       <c r="L16">
-        <v>-0.044871051</v>
+        <v>-0.2122522625214683</v>
       </c>
       <c r="M16">
-        <v>0.152162831</v>
+        <v>-0.09766339219853593</v>
       </c>
       <c r="N16">
-        <v>0.264317159</v>
+        <v>0.07815511282505004</v>
       </c>
       <c r="O16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="1">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B17">
-        <v>0.086281749</v>
+        <v>1.098824281425039</v>
       </c>
       <c r="C17">
-        <v>0.160537021</v>
+        <v>1.124544984094857</v>
       </c>
       <c r="D17">
-        <v>1.113430189</v>
+        <v>1.730050599012491</v>
       </c>
       <c r="E17">
-        <v>1.043262493</v>
+        <v>1.85323807668174</v>
       </c>
       <c r="F17">
-        <v>0.794527036</v>
+        <v>2.19314676580624</v>
       </c>
       <c r="G17">
-        <v>1.480132793</v>
+        <v>2.024663755796917</v>
       </c>
       <c r="H17">
-        <v>0.437978851</v>
+        <v>2.554541131790494</v>
       </c>
       <c r="I17">
-        <v>-0.162328318</v>
+        <v>2.318109608543673</v>
       </c>
       <c r="J17">
-        <v>0.655398369</v>
+        <v>2.100052046017395</v>
       </c>
       <c r="K17">
-        <v>0.8048442990000001</v>
+        <v>2.044557233732532</v>
       </c>
       <c r="L17">
-        <v>0.517525266</v>
+        <v>1.594573606845447</v>
       </c>
       <c r="M17">
-        <v>0.566780771</v>
+        <v>1.329427998478601</v>
       </c>
       <c r="N17">
-        <v>0.666223055</v>
+        <v>1.092029141150236</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="1">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B18">
-        <v>-0.919401809</v>
+        <v>-0.6057004064306782</v>
       </c>
       <c r="C18">
-        <v>-0.9502995000000001</v>
+        <v>-0.5377353754033299</v>
       </c>
       <c r="D18">
-        <v>0.198061398</v>
+        <v>0.06023393650398268</v>
       </c>
       <c r="E18">
-        <v>1.090531976</v>
+        <v>1.156450741882419</v>
       </c>
       <c r="F18">
-        <v>1.591912741</v>
+        <v>1.695659991481</v>
       </c>
       <c r="G18">
-        <v>1.419771212</v>
+        <v>0.5459799358931066</v>
       </c>
       <c r="H18">
-        <v>1.685263614</v>
+        <v>1.737616217432471</v>
       </c>
       <c r="I18">
-        <v>1.31493522</v>
+        <v>1.459572815406067</v>
       </c>
       <c r="J18">
-        <v>1.427681665</v>
+        <v>1.27574394030813</v>
       </c>
       <c r="K18">
-        <v>1.688971273</v>
+        <v>1.463114216622488</v>
       </c>
       <c r="L18">
-        <v>1.432602503</v>
+        <v>1.41933957798711</v>
       </c>
       <c r="M18">
-        <v>1.113826339</v>
+        <v>1.227404464743771</v>
       </c>
       <c r="N18">
-        <v>0.896996784</v>
+        <v>0.9388314252113402</v>
       </c>
       <c r="O18">
         <v>3</v>

</xml_diff>